<commit_message>
jobs now have working grouped/hidden attributes. now just gotta figure out how to tell that to the r/w
</commit_message>
<xml_diff>
--- a/ModSheet.xlsx
+++ b/ModSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gunk\Code\python\LCR2XL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FDC531-E353-4F17-B7CF-E21E4E039CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF45240-7734-4656-A528-5AF3D8735F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,11 +878,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.453125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
@@ -1242,7 +1242,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="str">
         <f>A14</f>
@@ -1298,7 +1298,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="str">
         <f>A14</f>
@@ -1324,7 +1324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="str">
         <f>A14</f>
@@ -1351,7 +1351,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="str">
         <f>A34</f>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="str">
         <f>A34</f>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="str">
         <f>A34</f>

</xml_diff>